<commit_message>
Update after RECOVERY was published on Lancet
</commit_message>
<xml_diff>
--- a/final_analyses/data/extracted-data.xlsx
+++ b/final_analyses/data/extracted-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/tocilizumab_reanalysis/final_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE1E252-104B-AA41-A38F-3FD5F2565967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D948E848-1202-E34B-A25C-6177C0E77A09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="-21140" windowWidth="19200" windowHeight="21140" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62B0DA3-8D81-B047-8685-9547CB3A5AEB}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1184,13 +1184,13 @@
         <v>31</v>
       </c>
       <c r="F17">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="G17">
         <v>935</v>
       </c>
       <c r="H17">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="I17">
         <v>933</v>
@@ -1213,13 +1213,13 @@
         <v>31</v>
       </c>
       <c r="F18">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="G18">
         <v>819</v>
       </c>
       <c r="H18">
-        <v>350</v>
+        <v>366</v>
       </c>
       <c r="I18">
         <v>867</v>
@@ -1242,13 +1242,13 @@
         <v>31</v>
       </c>
       <c r="F19">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G19">
         <v>268</v>
       </c>
       <c r="H19">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I19">
         <v>294</v>
@@ -1271,13 +1271,13 @@
         <v>31</v>
       </c>
       <c r="F20">
-        <v>668</v>
+        <v>697</v>
       </c>
       <c r="G20">
         <v>935</v>
       </c>
       <c r="H20">
-        <v>602</v>
+        <v>635</v>
       </c>
       <c r="I20">
         <v>933</v>
@@ -1300,13 +1300,13 @@
         <v>31</v>
       </c>
       <c r="F21">
-        <v>376</v>
+        <v>401</v>
       </c>
       <c r="G21">
         <v>819</v>
       </c>
       <c r="H21">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c r="I21">
         <v>867</v>
@@ -1329,7 +1329,7 @@
         <v>31</v>
       </c>
       <c r="F22">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G22">
         <v>268</v>
@@ -1358,13 +1358,13 @@
         <v>29</v>
       </c>
       <c r="F23">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G23">
         <v>668</v>
       </c>
       <c r="H23">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="I23">
         <v>660</v>
@@ -1387,13 +1387,13 @@
         <v>28</v>
       </c>
       <c r="F24">
-        <v>386</v>
+        <v>407</v>
       </c>
       <c r="G24">
         <v>1354</v>
       </c>
       <c r="H24">
-        <v>449</v>
+        <v>473</v>
       </c>
       <c r="I24">
         <v>1433</v>
@@ -1416,13 +1416,13 @@
         <v>29</v>
       </c>
       <c r="F25">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="G25">
         <v>668</v>
       </c>
       <c r="H25">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="I25">
         <v>660</v>
@@ -1445,13 +1445,13 @@
         <v>28</v>
       </c>
       <c r="F26">
-        <v>728</v>
+        <v>770</v>
       </c>
       <c r="G26">
         <v>1354</v>
       </c>
       <c r="H26">
-        <v>676</v>
+        <v>713</v>
       </c>
       <c r="I26">
         <v>1433</v>

</xml_diff>

<commit_message>
Changed oyxgen subgroup classification of CORIMUNO-19 from pooled to "simple oxygen only"
</commit_message>
<xml_diff>
--- a/final_analyses/data/extracted-data.xlsx
+++ b/final_analyses/data/extracted-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/tocilizumab_reanalysis/final_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D948E848-1202-E34B-A25C-6177C0E77A09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1816C693-490E-A24A-BA9E-4217737A259D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
+    <workbookView xWindow="1020" yWindow="-18820" windowWidth="28800" windowHeight="16520" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62B0DA3-8D81-B047-8685-9547CB3A5AEB}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,7 +827,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>31</v>
@@ -856,7 +856,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
update after third manuscript draft
</commit_message>
<xml_diff>
--- a/final_analyses/data/extracted-data.xlsx
+++ b/final_analyses/data/extracted-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/tocilizumab_reanalysis/final_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1816C693-490E-A24A-BA9E-4217737A259D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFC405D-EC41-7148-AA8D-38FC3ABEDB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-18820" windowWidth="28800" windowHeight="16520" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{C55321BB-4BEA-BA49-85B2-DAB23CE95272}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="84">
   <si>
     <t>trial</t>
   </si>
@@ -160,12 +160,6 @@
     <t xml:space="preserve">REMAP CAP included patients with either non-invasive or invasive mechanical ventilation. </t>
   </si>
   <si>
-    <t>Cochrane defines non-invasive ventilation or high flow oxygen = severe disease</t>
-  </si>
-  <si>
-    <t>Cochrane defines mechanical ventilation = critical disease</t>
-  </si>
-  <si>
     <t>REMAPCAP, tocilizumab arm: 101 (28.6%) in highflow oxygen, 147 (41.6%) non-invasive, 104 (29.5%) in invasive mechanical ventilation // control arm: 110 (27.4%), 169 (42%),121 (30%) (Table S1)</t>
   </si>
   <si>
@@ -188,20 +182,6 @@
   </si>
   <si>
     <t>CORIMUNO: discharge at D28 (eTable 9)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CORIMUNO death at D28 is different comparing Figure 2C vs. Abstract/Table 2/eTable8 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(CHECK THIS) I followed the latter</t>
-    </r>
   </si>
   <si>
     <t>REMAP CAP Table 2 "In‐hospital death — no./total no. (%)"</t>
@@ -329,6 +309,9 @@
   </si>
   <si>
     <t>pooled simple or non-invasive ventilation</t>
+  </si>
+  <si>
+    <t>CORIMUNO death at D28 (Abstract/Table 2/eTable8 )</t>
   </si>
 </sst>
 </file>
@@ -688,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62B0DA3-8D81-B047-8685-9547CB3A5AEB}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +781,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -1059,7 +1042,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
         <v>31</v>
@@ -1088,7 +1071,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
         <v>31</v>
@@ -1756,7 +1739,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1764,7 +1747,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1772,7 +1755,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1806,10 +1789,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1817,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1825,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1833,7 +1816,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1841,7 +1824,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1849,7 +1832,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1857,7 +1840,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1865,7 +1848,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1873,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1881,7 +1864,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1889,7 +1872,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1897,7 +1880,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1905,7 +1888,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1913,7 +1896,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1921,7 +1904,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1929,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1937,7 +1920,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1945,7 +1928,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1953,7 +1936,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1961,7 +1944,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1969,7 +1952,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1977,7 +1960,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1987,67 +1970,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044BBB06-1911-D145-AE5B-C873BBEA08D7}">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
@@ -2055,29 +2043,29 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
@@ -2085,39 +2073,24 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-    </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>